<commit_message>
Đánh giá lần 3.
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="PA3" sheetId="3" r:id="rId1"/>
-    <sheet name="PA" sheetId="5" r:id="rId2"/>
-    <sheet name="DanhGia" sheetId="6" r:id="rId3"/>
+    <sheet name="PA" sheetId="5" r:id="rId1"/>
+    <sheet name="DanhGia" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>0812506</t>
   </si>
@@ -33,27 +32,9 @@
     <t>0812531</t>
   </si>
   <si>
-    <t>Viết scenario</t>
-  </si>
-  <si>
-    <t>Thiết kế paper prototype "Tham quan nhà hàng"</t>
-  </si>
-  <si>
-    <t>Thiết kế computer prototype "Tìm kiếm"</t>
-  </si>
-  <si>
-    <t>Thiết kế computer prototype "Đặt bàn"</t>
-  </si>
-  <si>
-    <t>Đánh giá prototype</t>
-  </si>
-  <si>
     <t>MSSV</t>
   </si>
   <si>
-    <t>Công việc thực hiện</t>
-  </si>
-  <si>
     <t>PA1</t>
   </si>
   <si>
@@ -915,7 +896,36 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Đánh giá tổng quan lần 2</t>
+      <t xml:space="preserve">Đánh giá tổng quan lần 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá tổng quan lần 3</t>
     </r>
   </si>
   <si>
@@ -1032,7 +1042,36 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Đánh giá tổng quan lần 2</t>
+      <t xml:space="preserve">Đánh giá tổng quan lần 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá tổng quan lần 3</t>
     </r>
   </si>
   <si>
@@ -1178,7 +1217,36 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Đánh giá tổng quan lần 2</t>
+      <t xml:space="preserve">Đánh giá tổng quan lần 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá tổng quan lần 3</t>
     </r>
   </si>
   <si>
@@ -1324,7 +1392,36 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Đánh giá tổng quan lần 2</t>
+      <t xml:space="preserve">Đánh giá tổng quan lần 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá tổng quan lần 3</t>
     </r>
   </si>
   <si>
@@ -1432,7 +1529,36 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Đánh giá tổng quan lần 2</t>
+      <t xml:space="preserve">Đánh giá tổng quan lần 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá tổng quan lần 3</t>
     </r>
   </si>
 </sst>
@@ -1440,21 +1566,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1485,24 +1602,12 @@
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1538,31 +1643,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1859,123 +1951,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="3" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1990,105 +1965,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Cập nhật công việc đã làm.
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>0812506</t>
   </si>
@@ -35,18 +35,6 @@
     <t>MSSV</t>
   </si>
   <si>
-    <t>PA1</t>
-  </si>
-  <si>
-    <t>PA2</t>
-  </si>
-  <si>
-    <t>PA3</t>
-  </si>
-  <si>
-    <t>PA4</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1560,6 +1548,159 @@
       </rPr>
       <t>Đánh giá tổng quan lần 3</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tổng hợp câu hỏi khảo sát</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chọn câu hỏi khảo sát</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chụp hình và chú thích
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chọn câu hỏi khảo sát
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>PA1 (20/20)</t>
+  </si>
+  <si>
+    <t>PA2 (100/100)</t>
+  </si>
+  <si>
+    <t>PA3 (90/100)</t>
+  </si>
+  <si>
+    <t>PA4 (113+13/120+20)</t>
+  </si>
+  <si>
+    <t>PA5 (?/20+50)</t>
   </si>
 </sst>
 </file>
@@ -1951,9 +2092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1962,108 +2105,125 @@
     <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90">
+    <row r="2" spans="1:6" ht="90">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="75">
+    <row r="3" spans="1:6" ht="75">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90">
+    <row r="4" spans="1:6" ht="90">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:6" ht="90">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75">
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Đánh giá công việc hoàn tất.
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="PA" sheetId="5" r:id="rId1"/>
-    <sheet name="DanhGia" sheetId="6" r:id="rId2"/>
+    <sheet name="PA 1-5" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>0812506</t>
   </si>
@@ -1550,33 +1549,465 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tổng hợp câu hỏi khảo sát</t>
+    <t>PA1 (20/20)</t>
+  </si>
+  <si>
+    <t>PA2 (100/100)</t>
+  </si>
+  <si>
+    <t>PA3 (90/100)</t>
+  </si>
+  <si>
+    <t>PA4 (113+13/120+20)</t>
+  </si>
+  <si>
+    <t>PA5 (?/20+50)</t>
+  </si>
+  <si>
+    <t>Đánh giá</t>
+  </si>
+  <si>
+    <t>Nhận xét</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chọn câu hỏi khảo sát
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Khảo sát 3 người
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Review lại các tài liệu nộp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chọn câu hỏi khảo sát
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Khảo sát 2 người
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Review lại các tài liệu nộp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Khảo sát 2 người
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Review lại các tài liệu nộp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tổng hợp câu hỏi khảo sát
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Khảo sát 2 người
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Review lại các tài liệu nộp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chụp hình và chú thích
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chọn câu hỏi khảo sát
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Khảo sát 5 người
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thống kê kết quả khảo sát
+</t>
     </r>
     <r>
       <rPr>
@@ -1587,120 +2018,6 @@
       </rPr>
       <t/>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Chọn câu hỏi khảo sát</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Chụp hình và chú thích
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Chọn câu hỏi khảo sát
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <t>PA1 (20/20)</t>
-  </si>
-  <si>
-    <t>PA2 (100/100)</t>
-  </si>
-  <si>
-    <t>PA3 (90/100)</t>
-  </si>
-  <si>
-    <t>PA4 (113+13/120+20)</t>
-  </si>
-  <si>
-    <t>PA5 (?/20+50)</t>
   </si>
 </sst>
 </file>
@@ -2092,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2105,30 +2422,36 @@
     <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="90">
+    <row r="2" spans="1:8" ht="90">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2145,10 +2468,12 @@
         <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="75">
+    <row r="3" spans="1:8" ht="75">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2165,10 +2490,12 @@
         <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="90">
+    <row r="4" spans="1:8" ht="90">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2184,9 +2511,13 @@
       <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="90">
+    <row r="5" spans="1:8" ht="90">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2203,10 +2534,12 @@
         <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="75">
+    <row r="6" spans="1:8" ht="75">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2223,23 +2556,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>